<commit_message>
full function finish, bugs may exist
</commit_message>
<xml_diff>
--- a/io_matrix.xlsx
+++ b/io_matrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -53,13 +53,29 @@
   </si>
   <si>
     <t>gpio[6]</t>
+  </si>
+  <si>
+    <t>uart_tx</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>debug</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>debug[1]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>uart_rx</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,11 +713,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -775,6 +796,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -809,6 +831,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -984,28 +1007,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1019,13 +1047,16 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1034,6 +1065,15 @@
       </c>
       <c r="C3" t="s">
         <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>